<commit_message>
Update AHLE scenario parameters.xlsx
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ED3F97-6AC2-A54E-8091-C10139496D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F75541-D4AA-1E4A-A07A-BA142577E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
@@ -1092,9 +1092,6 @@
     <t>DM_in_feed</t>
   </si>
   <si>
-    <t>Lab_SR</t>
-  </si>
-  <si>
     <t>lab_non_health</t>
   </si>
   <si>
@@ -1186,6 +1183,9 @@
   </si>
   <si>
     <t>Rules for this to be read by the program</t>
+  </si>
+  <si>
+    <t>Labour</t>
   </si>
 </sst>
 </file>
@@ -1686,9 +1686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:BB121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO31" sqref="AO31:AO34"/>
+      <selection pane="topRight" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1733,7 +1733,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>107</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -3813,10 +3813,10 @@
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" t="s">
         <v>339</v>
-      </c>
-      <c r="B20" t="s">
-        <v>340</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -6022,43 +6022,43 @@
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E44" t="s">
+        <v>342</v>
+      </c>
+      <c r="F44" t="s">
         <v>343</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>344</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>345</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>346</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>347</v>
-      </c>
-      <c r="J44" t="s">
-        <v>348</v>
       </c>
       <c r="K44" s="6" t="s">
         <v>84</v>
       </c>
       <c r="L44" t="s">
+        <v>348</v>
+      </c>
+      <c r="M44" t="s">
         <v>349</v>
       </c>
-      <c r="M44" t="s">
+      <c r="N44" t="s">
         <v>350</v>
       </c>
-      <c r="N44" t="s">
+      <c r="O44" t="s">
         <v>351</v>
-      </c>
-      <c r="O44" t="s">
-        <v>352</v>
       </c>
       <c r="P44" s="4" t="s">
         <v>132</v>
@@ -6189,7 +6189,7 @@
         <v>85</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
@@ -6213,7 +6213,7 @@
         <v>85</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M45" t="s">
         <v>85</v>
@@ -6377,7 +6377,7 @@
         <v>85</v>
       </c>
       <c r="L46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>86</v>
@@ -7112,16 +7112,16 @@
         <v>97</v>
       </c>
       <c r="L55" t="s">
+        <v>352</v>
+      </c>
+      <c r="M55" t="s">
         <v>353</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>354</v>
       </c>
-      <c r="N55" t="s">
+      <c r="O55" t="s">
         <v>355</v>
-      </c>
-      <c r="O55" t="s">
-        <v>356</v>
       </c>
       <c r="P55" s="4" t="s">
         <v>136</v>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="63" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C63">
         <v>0.25</v>
@@ -11445,7 +11445,7 @@
     </row>
     <row r="108" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
-        <v>332</v>
+        <v>363</v>
       </c>
       <c r="C108" t="s">
         <v>105</v>
@@ -11606,7 +11606,7 @@
     </row>
     <row r="109" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -11854,7 +11854,7 @@
     </row>
     <row r="115" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B115" t="s">
         <v>70</v>
@@ -12066,7 +12066,7 @@
     </row>
     <row r="119" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -12269,37 +12269,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to code and cleaning scenario params
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC1103E-C311-9946-9B5B-B1FD902DED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E6F60-E1B6-154A-9C56-4CF88D2A87C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="6060" yWindow="500" windowWidth="21940" windowHeight="16300" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1584,12 +1584,6 @@
     <t>rpert(10000, (0.52+((0.3-0.52)*0.75)), (0.67+((1.8-0.67)*0.75)),  (0.60+((0.8-0.6)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (0.37+((0.25-0.37)*0.25)), (0.50+(1.2-0.5)*0.25)), (0.46+((0.85-0.46)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (0.37+((0.25-0.37)*0.5)), (0.50+(1.2-0.5)*0.5)), (0.46+((0.85-0.46)*0.5)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (0.37+((0.25-0.37)*0.75)), (0.50+((1.2-0.5)*0.75)), (0.46+((0.85-0.46)*0.75)))</t>
   </si>
   <si>
@@ -1917,24 +1911,6 @@
     <t>rtruncnorm(10000, (1+((6-1)*0.75)), (15+((20-15)*0.75)), (8.5+((11.8-8.5)*0.75)), 1.6)</t>
   </si>
   <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((16.5-15)*0.25), (11.7+(14-11.7)*0.25)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((16.5-15)*0.5), (11.7+(14-11.7)*0.5)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((16.5-15)*0.75), (11.7+(14-11.7)*0.75)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6-1)*0.25)), (15+((15.5-15)*0.25), (8.8+((13-8.8)*0.25)), 1.3)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6-1)*0.5)), (15+((15.5-15)*0.5), (8.8+((13-8.8)*0.5)), 1.3)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6-1)*0.75)), (15+((15.5-15)*0.75), (8.8+((13-8.8)*0.75)), 1.3)</t>
-  </si>
-  <si>
     <t>rtruncnorm(10000, (1+((7.5-1)*0.25)), (15+((24.5-15)*0.25)), (11.7+((13.2-11.7)*0.25)), 2.2)</t>
   </si>
   <si>
@@ -1944,33 +1920,6 @@
     <t>rtruncnorm(10000, (1+((7.5-1)*0.75)), (15+((24.5-15)*0.75)), (11.7+((13.2-11.7)*0.75)), 2.2)</t>
   </si>
   <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((21.5-15)*0.25)), (8.5+12.5-8.5*0.25)), sd = 1.6)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((21.5-15)*0.5)), (8.5+12.5-8.5*0.5)), sd = 1.6)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((21.5-15)*0.75)), (8.5+12.5-8.5*0.75)), sd = 1.6)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((7-1)*0.25)), (15+((17-15)*0.25), (11.7+(13.8-11.7)*0.25)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((7-1)*0.5)), (15+((17-15)*0.5), (11.7+(13.8-11.7)*0.5)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((7-1)*0.75)), (15+((17-15)*0.75), (11.7+(13.8-11.7)*0.75)), sd = 2.2)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((17-15)*0.25), (8.8+((13.8-8.8)*0.25)), 1.3)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((17-15)*0.5), (8.8+((13.8-8.8)*0.5)), 1.3)</t>
-  </si>
-  <si>
-    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((17-15)*0.75), (8.8+((13.8-8.8)*0.75)), 1.3)</t>
-  </si>
-  <si>
     <t>rnorm(10000, (21.1+((21.5-21.1)*0.25)), sd = 3.8)</t>
   </si>
   <si>
@@ -2052,15 +2001,6 @@
     <t>rnorm(10000, (28.6+((31.2-28.6)*0.75)), sd = 4.1)</t>
   </si>
   <si>
-    <t xml:space="preserve">rnorm(10000, (25.1+(35-25.1)*0.25)), sd = 0.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rnorm(10000, (25.1+(35-25.1)*0.5)), sd = 0.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rnorm(10000, (25.1+(35-25.1)*0.75)), sd = 0.2) </t>
-  </si>
-  <si>
     <t xml:space="preserve">rnorm(10000, (29.6+((29-29.6)*0.25)), sd = 0.7) </t>
   </si>
   <si>
@@ -2151,15 +2091,6 @@
     <t>rpert(10000, (925+((1366-925)*0.75)), (1483+((2191-1483)*0.75)), (1098+((1622-1098)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (1246+((1276+1246)*0.25)), (4300+((4402-4300)*0.25)), (2120+((2170-2120)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1246+((1276+1246)*0.5)), (4300+((4402-4300)*0.5)), (2120+((2170-2120)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1246+((1276+1246)*0.75)), (4300+((4402-4300)*0.75)), (2120+((2170-2120)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (1355+((2092-1355)*0.25)), (2158+((3332-2158)*0.25)), (1785+((2756-1758)*0.25)))</t>
   </si>
   <si>
@@ -2169,15 +2100,6 @@
     <t>rpert(10000, (1355+((2092-1355)*0.75)), (2158+((3332-2158)*0.75)), (1785+((2756-1758)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (1591+((1591-1591)*0.25)), (2417+((2417-2417*0.25)), (1836+((2417-1836)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1591+((1591-1591)*0.5)), (2417+((2417-2417*0.5)), (1836+((2417-1836)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1591+((1591-1591)*0.75)), (2417+((2417-2417*0.75)), (1836+((2417-1836)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (1065+((1388-1065)*0.25)), (2372+((3092-2372)*0.25)), (1695+((2210-1695)*0.25)))</t>
   </si>
   <si>
@@ -2187,15 +2109,6 @@
     <t>rpert(10000, (1065+((1388-1065)*0.75)), (2372+((3092-2372)*0.75)), (1695+((2210-1695)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (2400+((2637-2400)*0.25)), (4013+((4409-4013)*0.25)), (2890+(3175-2890)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (2400+((2637-2400)*0.5)), (4013+((4409-4013)*0.5)), (2890+(3175-2890)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (2400+((2637-2400)*0.75)), (4013+((4409-4013)*0.75)), (2890+(3175-2890)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (2140+((2038-2140)*0.25)), (4093+((5018-4093)*0.25)), (3210+((3333-3210)*0.25)))</t>
   </si>
   <si>
@@ -2205,15 +2118,6 @@
     <t>rpert(10000, (2140+((2038-2140)*0.75)), (4093+((5018-4093)*0.75)), (3210+((3333-3210)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (1663, 2687, (2051+((2687-2051)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1663, 2687, (2051+((2687-2051)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (1663, 2687, (2051+((2687-2051)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (1800+((1972-1800)*0.25)), (3600+((3944-3600)*0.25)), (2620+((2871-2620)*0.25)))</t>
   </si>
   <si>
@@ -2223,15 +2127,6 @@
     <t>rpert(10000, (1800+((1972-1800)*0.75)), (3600+((3944-3600)*0.75)), (2620+((2871-2620)*0.75)))</t>
   </si>
   <si>
-    <t>rpert(10000, (839+((947-839)*0.25)), (1676+(1891-1676)*0.25)), (1385+((1563-1385)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (839+((947-839)*0.5)), (1676+(1891-1676)*0.5)), (1385+((1563-1385)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, (839+((947-839)*0.75)), (1676+(1891-1676)*0.75)), (1385+((1563-1385)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (810+((1191-810)*0.25)), (1713+((2519-1713)*0.25)), (1266+((1862-1266)*0.25)))</t>
   </si>
   <si>
@@ -2277,15 +2172,6 @@
     <t xml:space="preserve">rpert(10000, (1355+((2222-1355)*0.75)), (3966+((6503-3966)*0.75)), (2459+((4032-2459)*0.75))) </t>
   </si>
   <si>
-    <t>rpert(10000, 1366, 2701, (1871+(2701-1871)*0.25)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, 1366, 2701, (1871+(2701-1871)*0.5)))</t>
-  </si>
-  <si>
-    <t>rpert(10000, 1366, 2701, (1871+(2701-1871)*0.75)))</t>
-  </si>
-  <si>
     <t>rpert(10000, (1100+((1476-1100)*0.25)), (2700+((3623-2700)*0.25)), (2011+((2699-2011)*0.25)))</t>
   </si>
   <si>
@@ -2329,6 +2215,120 @@
   </si>
   <si>
     <t>rpert(10000, (2330+((2692-2330)*0.75)), (5238+((6052-5238)*0.75)), (3796+((4386-3796)*0.75)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (0.37+((0.25-0.37)*0.25)), (0.50+((1.2-0.5)*0.25)), (0.46+((0.85-0.46)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (0.37+((0.25-0.37)*0.5)), (0.50+((1.2-0.5)*0.5)), (0.46+((0.85-0.46)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (839+((947-839)*0.25)), (1676+((1891-1676)*0.25)), (1385+((1563-1385)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (2400+((2637-2400)*0.25)), (4013+((4409-4013)*0.25)), (2890+((3175-2890)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (839+((947-839)*0.5)), (1676+((1891-1676)*0.5)), (1385+((1563-1385)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (2400+((2637-2400)*0.5)), (4013+((4409-4013)*0.5)), (2890+((3175-2890)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (839+((947-839)*0.75)), (1676+((1891-1676)*0.75)), (1385+((1563-1385)*0.75)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (2400+((2637-2400)*0.75)), (4013+((4409-4013)*0.75)), (2890+((3175-2890)*0.75)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1246+((1276-1246)*0.5)), (4300+((4402-4300)*0.5)), (2120+((2170-2120)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1246+((1276-1246)*0.25)), (4300+((4402-4300)*0.25)), (2120+((2170-2120)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1246+((1276-1246)*0.75)), (4300+((4402-4300)*0.75)), (2120+((2170-2120)*0.75)))</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((21.5-15)*0.75)), (8.5+((12.5-8.5)*0.75)), sd = 1.6)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((21.5-15)*0.5)), (8.5+((12.5-8.5)*0.5)), sd = 1.6)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((21.5-15)*0.25)), (8.5+((12.5-8.5)*0.25)), sd = 1.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnorm(10000, (25.1+((35-25.1)*0.25)), sd = 0.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnorm(10000, (25.1+((35-25.1)*0.5)), sd = 0.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnorm(10000, (25.1+((35-25.1)*0.75)), sd = 0.2) </t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((16.5-15)*0.25)), (11.7+((14-11.7)*0.25)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((16.5-15)*0.5)), (11.7+((14-11.7)*0.5)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((7-1)*0.5)), (15+((17-15)*0.5)), (11.7+((13.8-11.7)*0.5)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((16.5-15)*0.75)), (11.7+((14-11.7)*0.75)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((7-1)*0.75)), (15+((17-15)*0.75)), (11.7+((13.8-11.7)*0.75)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1366, 2701, (1871+((2701-1871)*0.75)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1663, 2687, (2051+((2687-2051)*0.5)))</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((7-1)*0.25)), (15+((17-15)*0.25)), (11.7+((13.8-11.7)*0.25)), sd = 2.2)</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1591+((1591-1591)*0.25)), (2417+((2417-2417)*0.25)), (1836+((2417-1836)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1591+((1591-1591)*0.5)), (2417+((2417-2417)*0.5)), (1836+((2417-1836)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1366, 2701, (1871+((2701-1871)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1366, 2701, (1871+((2701-1871)*0.5)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1663, 2687, (2051+((2687-2051)*0.25)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (1591+((1591-1591)*0.75)), (2417+((2417-2417)*0.75)), (1836+((2417-1836)*0.75)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 1663, 2687, (2051+((2687-2051)*0.75)))</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6-1)*0.25)), (15+((15.5-15)*0.25)), (8.8+((13-8.8)*0.25)), 1.3)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.25)), (15+((17-15)*0.25)), (8.8+((13.8-8.8)*0.25)), 1.3)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.5)), (15+((17-15)*0.5)), (8.8+((13.8-8.8)*0.5)), 1.3)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6-1)*0.5)), (15+((15.5-15)*0.5)), (8.8+((13-8.8)*0.5)), 1.3)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6-1)*0.75)), (15+((15.5-15)*0.75)), (8.8+((13-8.8)*0.75)), 1.3)</t>
+  </si>
+  <si>
+    <t>rtruncnorm(10000, (1+((6.5-1)*0.75)), (15+((17-15)*0.75)), (8.8+((13.8-8.8)*0.75)), 1.3)</t>
   </si>
 </sst>
 </file>
@@ -2405,7 +2405,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2460,6 +2460,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2482,7 +2488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2550,6 +2556,9 @@
     <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2866,9 +2875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:HR121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EA1" sqref="EA1:HR1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="HI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="HL60" sqref="HL60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2916,7 +2925,7 @@
     <col min="95" max="96" width="42.1640625" customWidth="1"/>
     <col min="97" max="108" width="18" customWidth="1"/>
     <col min="109" max="114" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="78.1640625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="53.1640625" customWidth="1"/>
     <col min="116" max="116" width="52.33203125" customWidth="1"/>
     <col min="117" max="117" width="78.1640625" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="52.33203125" customWidth="1"/>
@@ -2925,8 +2934,8 @@
     <col min="123" max="126" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="82.33203125" bestFit="1" customWidth="1"/>
     <col min="128" max="130" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19.1640625" customWidth="1"/>
-    <col min="132" max="132" width="17.5" customWidth="1"/>
+    <col min="131" max="131" width="28" customWidth="1"/>
+    <col min="132" max="132" width="56.83203125" customWidth="1"/>
     <col min="133" max="133" width="18" customWidth="1"/>
     <col min="134" max="134" width="18.5" customWidth="1"/>
     <col min="135" max="135" width="18" customWidth="1"/>
@@ -3362,292 +3371,292 @@
         <v>492</v>
       </c>
       <c r="EA1" s="37" t="s">
+        <v>503</v>
+      </c>
+      <c r="EB1" s="37" t="s">
+        <v>504</v>
+      </c>
+      <c r="EC1" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="EB1" s="37" t="s">
+      <c r="ED1" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="EC1" s="37" t="s">
+      <c r="EE1" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="ED1" s="37" t="s">
+      <c r="EF1" s="37" t="s">
         <v>508</v>
       </c>
-      <c r="EE1" s="37" t="s">
+      <c r="EG1" s="37" t="s">
         <v>509</v>
       </c>
-      <c r="EF1" s="37" t="s">
+      <c r="EH1" s="37" t="s">
         <v>510</v>
       </c>
-      <c r="EG1" s="37" t="s">
+      <c r="EI1" s="37" t="s">
         <v>511</v>
       </c>
-      <c r="EH1" s="37" t="s">
+      <c r="EJ1" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="EI1" s="37" t="s">
+      <c r="EK1" s="37" t="s">
         <v>513</v>
       </c>
-      <c r="EJ1" s="37" t="s">
+      <c r="EL1" s="37" t="s">
         <v>514</v>
       </c>
-      <c r="EK1" s="37" t="s">
+      <c r="EM1" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="EL1" s="37" t="s">
+      <c r="EN1" s="37" t="s">
         <v>516</v>
       </c>
-      <c r="EM1" s="37" t="s">
+      <c r="EO1" s="37" t="s">
         <v>517</v>
       </c>
-      <c r="EN1" s="37" t="s">
+      <c r="EP1" s="37" t="s">
         <v>518</v>
       </c>
-      <c r="EO1" s="37" t="s">
+      <c r="EQ1" s="37" t="s">
         <v>519</v>
       </c>
-      <c r="EP1" s="37" t="s">
+      <c r="ER1" s="37" t="s">
         <v>520</v>
       </c>
-      <c r="EQ1" s="37" t="s">
+      <c r="ES1" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="ER1" s="37" t="s">
+      <c r="ET1" s="37" t="s">
         <v>522</v>
       </c>
-      <c r="ES1" s="37" t="s">
+      <c r="EU1" s="37" t="s">
         <v>523</v>
       </c>
-      <c r="ET1" s="37" t="s">
+      <c r="EV1" s="37" t="s">
         <v>524</v>
       </c>
-      <c r="EU1" s="37" t="s">
+      <c r="EW1" s="37" t="s">
         <v>525</v>
       </c>
-      <c r="EV1" s="37" t="s">
+      <c r="EX1" s="37" t="s">
         <v>526</v>
       </c>
-      <c r="EW1" s="37" t="s">
+      <c r="EY1" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="EX1" s="37" t="s">
+      <c r="EZ1" s="37" t="s">
         <v>528</v>
       </c>
-      <c r="EY1" s="37" t="s">
+      <c r="FA1" s="37" t="s">
         <v>529</v>
       </c>
-      <c r="EZ1" s="37" t="s">
+      <c r="FB1" s="37" t="s">
         <v>530</v>
       </c>
-      <c r="FA1" s="37" t="s">
+      <c r="FC1" s="37" t="s">
         <v>531</v>
       </c>
-      <c r="FB1" s="37" t="s">
+      <c r="FD1" s="37" t="s">
         <v>532</v>
       </c>
-      <c r="FC1" s="37" t="s">
+      <c r="FE1" s="37" t="s">
         <v>533</v>
       </c>
-      <c r="FD1" s="37" t="s">
+      <c r="FF1" s="37" t="s">
         <v>534</v>
       </c>
-      <c r="FE1" s="37" t="s">
+      <c r="FG1" s="37" t="s">
         <v>535</v>
       </c>
-      <c r="FF1" s="37" t="s">
+      <c r="FH1" s="37" t="s">
         <v>536</v>
       </c>
-      <c r="FG1" s="37" t="s">
+      <c r="FI1" s="37" t="s">
         <v>537</v>
       </c>
-      <c r="FH1" s="37" t="s">
+      <c r="FJ1" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="FI1" s="37" t="s">
+      <c r="FK1" s="37" t="s">
         <v>539</v>
       </c>
-      <c r="FJ1" s="37" t="s">
+      <c r="FL1" s="37" t="s">
         <v>540</v>
       </c>
-      <c r="FK1" s="37" t="s">
+      <c r="FM1" s="37" t="s">
         <v>541</v>
       </c>
-      <c r="FL1" s="37" t="s">
+      <c r="FN1" s="37" t="s">
         <v>542</v>
       </c>
-      <c r="FM1" s="37" t="s">
+      <c r="FO1" s="37" t="s">
         <v>543</v>
       </c>
-      <c r="FN1" s="37" t="s">
+      <c r="FP1" s="37" t="s">
         <v>544</v>
       </c>
-      <c r="FO1" s="37" t="s">
+      <c r="FQ1" s="37" t="s">
         <v>545</v>
       </c>
-      <c r="FP1" s="37" t="s">
+      <c r="FR1" s="37" t="s">
         <v>546</v>
       </c>
-      <c r="FQ1" s="37" t="s">
+      <c r="FS1" s="37" t="s">
         <v>547</v>
       </c>
-      <c r="FR1" s="37" t="s">
+      <c r="FT1" s="37" t="s">
         <v>548</v>
       </c>
-      <c r="FS1" s="37" t="s">
+      <c r="FU1" s="37" t="s">
         <v>549</v>
       </c>
-      <c r="FT1" s="37" t="s">
+      <c r="FV1" s="37" t="s">
         <v>550</v>
       </c>
-      <c r="FU1" s="37" t="s">
+      <c r="FW1" s="37" t="s">
         <v>551</v>
       </c>
-      <c r="FV1" s="37" t="s">
+      <c r="FX1" s="37" t="s">
         <v>552</v>
       </c>
-      <c r="FW1" s="37" t="s">
+      <c r="FY1" s="37" t="s">
         <v>553</v>
       </c>
-      <c r="FX1" s="37" t="s">
+      <c r="FZ1" s="37" t="s">
         <v>554</v>
       </c>
-      <c r="FY1" s="37" t="s">
+      <c r="GA1" s="37" t="s">
         <v>555</v>
       </c>
-      <c r="FZ1" s="37" t="s">
+      <c r="GB1" s="37" t="s">
         <v>556</v>
       </c>
-      <c r="GA1" s="37" t="s">
+      <c r="GC1" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="GB1" s="37" t="s">
+      <c r="GD1" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="GC1" s="37" t="s">
+      <c r="GE1" s="37" t="s">
         <v>559</v>
       </c>
-      <c r="GD1" s="37" t="s">
+      <c r="GF1" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="GE1" s="37" t="s">
+      <c r="GG1" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="GF1" s="37" t="s">
+      <c r="GH1" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="GG1" s="37" t="s">
+      <c r="GI1" s="37" t="s">
         <v>563</v>
       </c>
-      <c r="GH1" s="37" t="s">
+      <c r="GJ1" s="37" t="s">
         <v>564</v>
       </c>
-      <c r="GI1" s="37" t="s">
+      <c r="GK1" s="37" t="s">
         <v>565</v>
       </c>
-      <c r="GJ1" s="37" t="s">
+      <c r="GL1" s="37" t="s">
         <v>566</v>
       </c>
-      <c r="GK1" s="37" t="s">
+      <c r="GM1" s="37" t="s">
         <v>567</v>
       </c>
-      <c r="GL1" s="37" t="s">
+      <c r="GN1" s="37" t="s">
         <v>568</v>
       </c>
-      <c r="GM1" s="37" t="s">
+      <c r="GO1" s="37" t="s">
         <v>569</v>
       </c>
-      <c r="GN1" s="37" t="s">
+      <c r="GP1" s="37" t="s">
         <v>570</v>
       </c>
-      <c r="GO1" s="37" t="s">
+      <c r="GQ1" s="37" t="s">
         <v>571</v>
       </c>
-      <c r="GP1" s="37" t="s">
+      <c r="GR1" s="37" t="s">
         <v>572</v>
       </c>
-      <c r="GQ1" s="37" t="s">
+      <c r="GS1" s="37" t="s">
         <v>573</v>
       </c>
-      <c r="GR1" s="37" t="s">
+      <c r="GT1" s="37" t="s">
         <v>574</v>
       </c>
-      <c r="GS1" s="37" t="s">
+      <c r="GU1" s="37" t="s">
         <v>575</v>
       </c>
-      <c r="GT1" s="37" t="s">
+      <c r="GV1" s="37" t="s">
         <v>576</v>
       </c>
-      <c r="GU1" s="37" t="s">
+      <c r="GW1" s="37" t="s">
         <v>577</v>
       </c>
-      <c r="GV1" s="37" t="s">
+      <c r="GX1" s="37" t="s">
         <v>578</v>
       </c>
-      <c r="GW1" s="37" t="s">
+      <c r="GY1" s="37" t="s">
         <v>579</v>
       </c>
-      <c r="GX1" s="37" t="s">
+      <c r="GZ1" s="37" t="s">
         <v>580</v>
       </c>
-      <c r="GY1" s="37" t="s">
+      <c r="HA1" s="37" t="s">
         <v>581</v>
       </c>
-      <c r="GZ1" s="37" t="s">
+      <c r="HB1" s="37" t="s">
         <v>582</v>
       </c>
-      <c r="HA1" s="37" t="s">
+      <c r="HC1" s="37" t="s">
         <v>583</v>
       </c>
-      <c r="HB1" s="37" t="s">
+      <c r="HD1" s="37" t="s">
         <v>584</v>
       </c>
-      <c r="HC1" s="37" t="s">
+      <c r="HE1" s="37" t="s">
         <v>585</v>
       </c>
-      <c r="HD1" s="37" t="s">
+      <c r="HF1" s="37" t="s">
         <v>586</v>
       </c>
-      <c r="HE1" s="37" t="s">
+      <c r="HG1" s="37" t="s">
         <v>587</v>
       </c>
-      <c r="HF1" s="37" t="s">
+      <c r="HH1" s="37" t="s">
         <v>588</v>
       </c>
-      <c r="HG1" s="37" t="s">
+      <c r="HI1" s="37" t="s">
         <v>589</v>
       </c>
-      <c r="HH1" s="37" t="s">
+      <c r="HJ1" s="37" t="s">
         <v>590</v>
       </c>
-      <c r="HI1" s="37" t="s">
+      <c r="HK1" s="37" t="s">
         <v>591</v>
       </c>
-      <c r="HJ1" s="37" t="s">
+      <c r="HL1" s="37" t="s">
         <v>592</v>
       </c>
-      <c r="HK1" s="37" t="s">
+      <c r="HM1" s="37" t="s">
         <v>593</v>
       </c>
-      <c r="HL1" s="37" t="s">
+      <c r="HN1" s="37" t="s">
         <v>594</v>
       </c>
-      <c r="HM1" s="37" t="s">
+      <c r="HO1" s="37" t="s">
         <v>595</v>
       </c>
-      <c r="HN1" s="37" t="s">
+      <c r="HP1" s="37" t="s">
         <v>596</v>
       </c>
-      <c r="HO1" s="37" t="s">
+      <c r="HQ1" s="37" t="s">
         <v>597</v>
       </c>
-      <c r="HP1" s="37" t="s">
+      <c r="HR1" s="37" t="s">
         <v>598</v>
-      </c>
-      <c r="HQ1" s="37" t="s">
-        <v>599</v>
-      </c>
-      <c r="HR1" s="37" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="2" spans="1:226" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9744,37 +9753,37 @@
         <v>76</v>
       </c>
       <c r="DO15" s="33" t="s">
+        <v>707</v>
+      </c>
+      <c r="DP15" s="33" t="s">
+        <v>708</v>
+      </c>
+      <c r="DQ15" s="33" t="s">
         <v>496</v>
-      </c>
-      <c r="DP15" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="DQ15" s="33" t="s">
-        <v>498</v>
       </c>
       <c r="DR15" s="19" t="s">
         <v>129</v>
       </c>
       <c r="DS15" s="34" t="s">
+        <v>497</v>
+      </c>
+      <c r="DT15" s="34" t="s">
+        <v>498</v>
+      </c>
+      <c r="DU15" s="34" t="s">
         <v>499</v>
-      </c>
-      <c r="DT15" s="34" t="s">
-        <v>500</v>
-      </c>
-      <c r="DU15" s="34" t="s">
-        <v>501</v>
       </c>
       <c r="DV15" s="18" t="s">
         <v>209</v>
       </c>
       <c r="DW15" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="DX15" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="DY15" s="22" t="s">
         <v>502</v>
-      </c>
-      <c r="DX15" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="DY15" s="22" t="s">
-        <v>504</v>
       </c>
       <c r="DZ15" s="20" t="s">
         <v>231</v>
@@ -19464,7 +19473,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="FW38" s="12">
-        <v>2.0833333333333332E-2</v>
+        <v>2.0833000000000001E-2</v>
       </c>
       <c r="FX38" s="12">
         <v>2.0833333333333332E-2</v>
@@ -20194,7 +20203,7 @@
         <v>221</v>
       </c>
       <c r="EA43" s="22" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="EB43" s="35" t="s">
         <v>82</v>
@@ -20212,7 +20221,7 @@
         <v>82</v>
       </c>
       <c r="EG43" s="22" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="EH43" s="35" t="s">
         <v>82</v>
@@ -20230,7 +20239,7 @@
         <v>82</v>
       </c>
       <c r="EM43" s="22" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="EN43" s="35" t="s">
         <v>82</v>
@@ -20266,7 +20275,7 @@
         <v>82</v>
       </c>
       <c r="EY43" s="33" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="EZ43" s="36" t="s">
         <v>120</v>
@@ -20284,7 +20293,7 @@
         <v>120</v>
       </c>
       <c r="FE43" s="33" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="FF43" s="36" t="s">
         <v>120</v>
@@ -20302,7 +20311,7 @@
         <v>120</v>
       </c>
       <c r="FK43" s="33" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="FL43" s="36" t="s">
         <v>120</v>
@@ -20338,7 +20347,7 @@
         <v>120</v>
       </c>
       <c r="FW43" s="22" t="s">
-        <v>607</v>
+        <v>724</v>
       </c>
       <c r="FX43" t="s">
         <v>82</v>
@@ -20356,7 +20365,7 @@
         <v>82</v>
       </c>
       <c r="GC43" s="22" t="s">
-        <v>608</v>
+        <v>725</v>
       </c>
       <c r="GD43" t="s">
         <v>82</v>
@@ -20374,7 +20383,7 @@
         <v>82</v>
       </c>
       <c r="GI43" s="22" t="s">
-        <v>609</v>
+        <v>727</v>
       </c>
       <c r="GJ43" t="s">
         <v>82</v>
@@ -20410,7 +20419,7 @@
         <v>82</v>
       </c>
       <c r="GU43" s="41" t="s">
-        <v>610</v>
+        <v>739</v>
       </c>
       <c r="GV43" s="22" t="s">
         <v>221</v>
@@ -20428,7 +20437,7 @@
         <v>221</v>
       </c>
       <c r="HA43" s="41" t="s">
-        <v>611</v>
+        <v>742</v>
       </c>
       <c r="HB43" s="22" t="s">
         <v>221</v>
@@ -20446,7 +20455,7 @@
         <v>221</v>
       </c>
       <c r="HG43" s="41" t="s">
-        <v>612</v>
+        <v>743</v>
       </c>
       <c r="HH43" s="22" t="s">
         <v>221</v>
@@ -20877,7 +20886,7 @@
         <v>288</v>
       </c>
       <c r="EB44" s="22" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="EC44" s="35" t="s">
         <v>288</v>
@@ -20895,7 +20904,7 @@
         <v>288</v>
       </c>
       <c r="EH44" s="22" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="EI44" s="35" t="s">
         <v>288</v>
@@ -20913,7 +20922,7 @@
         <v>288</v>
       </c>
       <c r="EN44" s="22" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="EO44" s="35" t="s">
         <v>288</v>
@@ -20949,7 +20958,7 @@
         <v>120</v>
       </c>
       <c r="EZ44" s="33" t="s">
-        <v>616</v>
+        <v>720</v>
       </c>
       <c r="FA44" s="36" t="s">
         <v>120</v>
@@ -20967,7 +20976,7 @@
         <v>120</v>
       </c>
       <c r="FF44" s="33" t="s">
-        <v>617</v>
+        <v>719</v>
       </c>
       <c r="FG44" s="36" t="s">
         <v>120</v>
@@ -20985,7 +20994,7 @@
         <v>120</v>
       </c>
       <c r="FL44" s="33" t="s">
-        <v>618</v>
+        <v>718</v>
       </c>
       <c r="FM44" s="36" t="s">
         <v>120</v>
@@ -21021,7 +21030,7 @@
         <v>82</v>
       </c>
       <c r="FX44" s="22" t="s">
-        <v>619</v>
+        <v>731</v>
       </c>
       <c r="FY44" t="s">
         <v>82</v>
@@ -21039,7 +21048,7 @@
         <v>82</v>
       </c>
       <c r="GD44" s="22" t="s">
-        <v>620</v>
+        <v>726</v>
       </c>
       <c r="GE44" t="s">
         <v>82</v>
@@ -21057,7 +21066,7 @@
         <v>82</v>
       </c>
       <c r="GJ44" s="22" t="s">
-        <v>621</v>
+        <v>728</v>
       </c>
       <c r="GK44" t="s">
         <v>82</v>
@@ -21093,7 +21102,7 @@
         <v>221</v>
       </c>
       <c r="GV44" s="41" t="s">
-        <v>622</v>
+        <v>740</v>
       </c>
       <c r="GW44" s="22" t="s">
         <v>221</v>
@@ -21111,7 +21120,7 @@
         <v>221</v>
       </c>
       <c r="HB44" s="41" t="s">
-        <v>623</v>
+        <v>741</v>
       </c>
       <c r="HC44" s="22" t="s">
         <v>221</v>
@@ -21129,7 +21138,7 @@
         <v>221</v>
       </c>
       <c r="HH44" s="41" t="s">
-        <v>624</v>
+        <v>744</v>
       </c>
       <c r="HI44" s="22" t="s">
         <v>221</v>
@@ -21560,7 +21569,7 @@
         <v>85</v>
       </c>
       <c r="EC45" s="22" t="s">
-        <v>625</v>
+        <v>608</v>
       </c>
       <c r="ED45" s="35" t="s">
         <v>85</v>
@@ -21578,7 +21587,7 @@
         <v>85</v>
       </c>
       <c r="EI45" s="22" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
       <c r="EJ45" s="35" t="s">
         <v>85</v>
@@ -21596,7 +21605,7 @@
         <v>85</v>
       </c>
       <c r="EO45" s="22" t="s">
-        <v>627</v>
+        <v>610</v>
       </c>
       <c r="EP45" s="35" t="s">
         <v>85</v>
@@ -21632,7 +21641,7 @@
         <v>121</v>
       </c>
       <c r="FA45" s="33" t="s">
-        <v>628</v>
+        <v>611</v>
       </c>
       <c r="FB45" s="36" t="s">
         <v>121</v>
@@ -21650,7 +21659,7 @@
         <v>121</v>
       </c>
       <c r="FG45" s="33" t="s">
-        <v>629</v>
+        <v>612</v>
       </c>
       <c r="FH45" s="36" t="s">
         <v>121</v>
@@ -21668,7 +21677,7 @@
         <v>121</v>
       </c>
       <c r="FM45" s="33" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
       <c r="FN45" s="36" t="s">
         <v>121</v>
@@ -21704,7 +21713,7 @@
         <v>203</v>
       </c>
       <c r="FY45" s="22" t="s">
-        <v>631</v>
+        <v>614</v>
       </c>
       <c r="FZ45" t="s">
         <v>203</v>
@@ -21722,7 +21731,7 @@
         <v>203</v>
       </c>
       <c r="GE45" s="22" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
       <c r="GF45" t="s">
         <v>203</v>
@@ -21740,7 +21749,7 @@
         <v>203</v>
       </c>
       <c r="GK45" s="22" t="s">
-        <v>633</v>
+        <v>616</v>
       </c>
       <c r="GL45" t="s">
         <v>203</v>
@@ -21776,7 +21785,7 @@
         <v>222</v>
       </c>
       <c r="GW45" s="41" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
       <c r="GX45" s="22" t="s">
         <v>222</v>
@@ -21794,7 +21803,7 @@
         <v>222</v>
       </c>
       <c r="HC45" s="41" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
       <c r="HD45" s="22" t="s">
         <v>222</v>
@@ -21812,7 +21821,7 @@
         <v>222</v>
       </c>
       <c r="HI45" s="41" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
       <c r="HJ45" s="22" t="s">
         <v>222</v>
@@ -22243,7 +22252,7 @@
         <v>85</v>
       </c>
       <c r="ED46" s="22" t="s">
-        <v>637</v>
+        <v>620</v>
       </c>
       <c r="EE46" s="35" t="s">
         <v>85</v>
@@ -22261,7 +22270,7 @@
         <v>85</v>
       </c>
       <c r="EJ46" s="22" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="EK46" s="35" t="s">
         <v>85</v>
@@ -22279,7 +22288,7 @@
         <v>85</v>
       </c>
       <c r="EP46" s="22" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
       <c r="EQ46" s="35" t="s">
         <v>85</v>
@@ -22315,7 +22324,7 @@
         <v>121</v>
       </c>
       <c r="FB46" s="33" t="s">
-        <v>640</v>
+        <v>623</v>
       </c>
       <c r="FC46" s="36" t="s">
         <v>121</v>
@@ -22333,7 +22342,7 @@
         <v>121</v>
       </c>
       <c r="FH46" s="33" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="FI46" s="36" t="s">
         <v>121</v>
@@ -22351,7 +22360,7 @@
         <v>121</v>
       </c>
       <c r="FN46" s="33" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
       <c r="FO46" s="36" t="s">
         <v>121</v>
@@ -22387,7 +22396,7 @@
         <v>203</v>
       </c>
       <c r="FZ46" s="22" t="s">
-        <v>643</v>
+        <v>626</v>
       </c>
       <c r="GA46" t="s">
         <v>203</v>
@@ -22405,7 +22414,7 @@
         <v>203</v>
       </c>
       <c r="GF46" s="22" t="s">
-        <v>644</v>
+        <v>627</v>
       </c>
       <c r="GG46" t="s">
         <v>203</v>
@@ -22423,7 +22432,7 @@
         <v>203</v>
       </c>
       <c r="GL46" s="22" t="s">
-        <v>645</v>
+        <v>628</v>
       </c>
       <c r="GM46" t="s">
         <v>203</v>
@@ -22459,7 +22468,7 @@
         <v>222</v>
       </c>
       <c r="GX46" s="41" t="s">
-        <v>646</v>
+        <v>629</v>
       </c>
       <c r="GY46" s="22" t="s">
         <v>222</v>
@@ -22477,7 +22486,7 @@
         <v>222</v>
       </c>
       <c r="HD46" s="41" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="HE46" s="22" t="s">
         <v>222</v>
@@ -22495,7 +22504,7 @@
         <v>222</v>
       </c>
       <c r="HJ46" s="41" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="HK46" s="22" t="s">
         <v>222</v>
@@ -22926,7 +22935,7 @@
         <v>87</v>
       </c>
       <c r="EE47" s="22" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="EF47" s="35" t="s">
         <v>87</v>
@@ -22944,7 +22953,7 @@
         <v>87</v>
       </c>
       <c r="EK47" s="22" t="s">
-        <v>650</v>
+        <v>633</v>
       </c>
       <c r="EL47" s="35" t="s">
         <v>87</v>
@@ -22962,7 +22971,7 @@
         <v>87</v>
       </c>
       <c r="EQ47" s="22" t="s">
-        <v>651</v>
+        <v>634</v>
       </c>
       <c r="ER47" s="35" t="s">
         <v>87</v>
@@ -22998,7 +23007,7 @@
         <v>122</v>
       </c>
       <c r="FC47" s="33" t="s">
-        <v>652</v>
+        <v>721</v>
       </c>
       <c r="FD47" s="36" t="s">
         <v>122</v>
@@ -23016,7 +23025,7 @@
         <v>122</v>
       </c>
       <c r="FI47" s="33" t="s">
-        <v>653</v>
+        <v>722</v>
       </c>
       <c r="FJ47" s="36" t="s">
         <v>122</v>
@@ -23034,7 +23043,7 @@
         <v>122</v>
       </c>
       <c r="FO47" s="33" t="s">
-        <v>654</v>
+        <v>723</v>
       </c>
       <c r="FP47" s="36" t="s">
         <v>122</v>
@@ -23070,7 +23079,7 @@
         <v>204</v>
       </c>
       <c r="GA47" s="22" t="s">
-        <v>655</v>
+        <v>635</v>
       </c>
       <c r="GB47" t="s">
         <v>204</v>
@@ -23088,7 +23097,7 @@
         <v>204</v>
       </c>
       <c r="GG47" s="22" t="s">
-        <v>656</v>
+        <v>636</v>
       </c>
       <c r="GH47" t="s">
         <v>204</v>
@@ -23106,7 +23115,7 @@
         <v>204</v>
       </c>
       <c r="GM47" s="22" t="s">
-        <v>657</v>
+        <v>637</v>
       </c>
       <c r="GN47" t="s">
         <v>204</v>
@@ -23142,7 +23151,7 @@
         <v>223</v>
       </c>
       <c r="GY47" s="41" t="s">
-        <v>658</v>
+        <v>638</v>
       </c>
       <c r="GZ47" s="22" t="s">
         <v>223</v>
@@ -23160,7 +23169,7 @@
         <v>223</v>
       </c>
       <c r="HE47" s="41" t="s">
-        <v>659</v>
+        <v>639</v>
       </c>
       <c r="HF47" s="22" t="s">
         <v>223</v>
@@ -23178,7 +23187,7 @@
         <v>223</v>
       </c>
       <c r="HK47" s="41" t="s">
-        <v>660</v>
+        <v>640</v>
       </c>
       <c r="HL47" s="22" t="s">
         <v>223</v>
@@ -23609,7 +23618,7 @@
         <v>88</v>
       </c>
       <c r="EF48" s="22" t="s">
-        <v>661</v>
+        <v>641</v>
       </c>
       <c r="EG48" s="35" t="s">
         <v>88</v>
@@ -23627,7 +23636,7 @@
         <v>88</v>
       </c>
       <c r="EL48" s="22" t="s">
-        <v>662</v>
+        <v>642</v>
       </c>
       <c r="EM48" s="35" t="s">
         <v>88</v>
@@ -23645,7 +23654,7 @@
         <v>88</v>
       </c>
       <c r="ER48" s="22" t="s">
-        <v>663</v>
+        <v>643</v>
       </c>
       <c r="ES48" s="35" t="s">
         <v>88</v>
@@ -23681,7 +23690,7 @@
         <v>123</v>
       </c>
       <c r="FD48" s="33" t="s">
-        <v>664</v>
+        <v>644</v>
       </c>
       <c r="FE48" s="36" t="s">
         <v>123</v>
@@ -23699,7 +23708,7 @@
         <v>123</v>
       </c>
       <c r="FJ48" s="33" t="s">
-        <v>665</v>
+        <v>645</v>
       </c>
       <c r="FK48" s="36" t="s">
         <v>123</v>
@@ -23717,7 +23726,7 @@
         <v>123</v>
       </c>
       <c r="FP48" s="33" t="s">
-        <v>666</v>
+        <v>646</v>
       </c>
       <c r="FQ48" s="36" t="s">
         <v>123</v>
@@ -23753,7 +23762,7 @@
         <v>205</v>
       </c>
       <c r="GB48" s="22" t="s">
-        <v>667</v>
+        <v>647</v>
       </c>
       <c r="GC48" t="s">
         <v>205</v>
@@ -23771,7 +23780,7 @@
         <v>205</v>
       </c>
       <c r="GH48" s="22" t="s">
-        <v>668</v>
+        <v>648</v>
       </c>
       <c r="GI48" t="s">
         <v>205</v>
@@ -23789,7 +23798,7 @@
         <v>205</v>
       </c>
       <c r="GN48" s="22" t="s">
-        <v>669</v>
+        <v>649</v>
       </c>
       <c r="GO48" t="s">
         <v>205</v>
@@ -23825,7 +23834,7 @@
         <v>223</v>
       </c>
       <c r="GZ48" s="41" t="s">
-        <v>670</v>
+        <v>650</v>
       </c>
       <c r="HA48" s="22" t="s">
         <v>223</v>
@@ -23843,7 +23852,7 @@
         <v>223</v>
       </c>
       <c r="HF48" s="41" t="s">
-        <v>671</v>
+        <v>651</v>
       </c>
       <c r="HG48" s="22" t="s">
         <v>223</v>
@@ -23861,7 +23870,7 @@
         <v>223</v>
       </c>
       <c r="HL48" s="41" t="s">
-        <v>672</v>
+        <v>652</v>
       </c>
       <c r="HM48" s="22" t="s">
         <v>223</v>
@@ -25198,7 +25207,7 @@
         <v>343</v>
       </c>
       <c r="EA55" s="22" t="s">
-        <v>673</v>
+        <v>653</v>
       </c>
       <c r="EB55" s="30" t="s">
         <v>310</v>
@@ -25216,7 +25225,7 @@
         <v>310</v>
       </c>
       <c r="EG55" s="22" t="s">
-        <v>674</v>
+        <v>654</v>
       </c>
       <c r="EH55" s="30" t="s">
         <v>310</v>
@@ -25234,7 +25243,7 @@
         <v>310</v>
       </c>
       <c r="EM55" s="22" t="s">
-        <v>675</v>
+        <v>655</v>
       </c>
       <c r="EN55" s="30" t="s">
         <v>310</v>
@@ -25270,7 +25279,7 @@
         <v>310</v>
       </c>
       <c r="EY55" s="33" t="s">
-        <v>676</v>
+        <v>656</v>
       </c>
       <c r="EZ55" s="4" t="s">
         <v>321</v>
@@ -25288,7 +25297,7 @@
         <v>321</v>
       </c>
       <c r="FE55" s="33" t="s">
-        <v>677</v>
+        <v>657</v>
       </c>
       <c r="FF55" s="4" t="s">
         <v>321</v>
@@ -25306,7 +25315,7 @@
         <v>321</v>
       </c>
       <c r="FK55" s="33" t="s">
-        <v>678</v>
+        <v>658</v>
       </c>
       <c r="FL55" s="4" t="s">
         <v>321</v>
@@ -25342,7 +25351,7 @@
         <v>321</v>
       </c>
       <c r="FW55" s="22" t="s">
-        <v>679</v>
+        <v>659</v>
       </c>
       <c r="FX55" t="s">
         <v>332</v>
@@ -25360,7 +25369,7 @@
         <v>332</v>
       </c>
       <c r="GC55" s="22" t="s">
-        <v>680</v>
+        <v>660</v>
       </c>
       <c r="GD55" t="s">
         <v>332</v>
@@ -25378,7 +25387,7 @@
         <v>332</v>
       </c>
       <c r="GI55" s="22" t="s">
-        <v>681</v>
+        <v>661</v>
       </c>
       <c r="GJ55" t="s">
         <v>332</v>
@@ -25414,7 +25423,7 @@
         <v>332</v>
       </c>
       <c r="GU55" s="41" t="s">
-        <v>682</v>
+        <v>662</v>
       </c>
       <c r="GV55" s="22" t="s">
         <v>343</v>
@@ -25432,7 +25441,7 @@
         <v>343</v>
       </c>
       <c r="HA55" s="41" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
       <c r="HB55" s="22" t="s">
         <v>343</v>
@@ -25450,7 +25459,7 @@
         <v>343</v>
       </c>
       <c r="HG55" s="41" t="s">
-        <v>684</v>
+        <v>664</v>
       </c>
       <c r="HH55" s="22" t="s">
         <v>343</v>
@@ -25884,7 +25893,7 @@
         <v>312</v>
       </c>
       <c r="EC56" s="22" t="s">
-        <v>685</v>
+        <v>716</v>
       </c>
       <c r="ED56" s="30" t="s">
         <v>312</v>
@@ -25902,7 +25911,7 @@
         <v>312</v>
       </c>
       <c r="EI56" s="22" t="s">
-        <v>686</v>
+        <v>715</v>
       </c>
       <c r="EJ56" s="30" t="s">
         <v>312</v>
@@ -25920,7 +25929,7 @@
         <v>312</v>
       </c>
       <c r="EO56" s="22" t="s">
-        <v>687</v>
+        <v>717</v>
       </c>
       <c r="EP56" s="30" t="s">
         <v>312</v>
@@ -25956,7 +25965,7 @@
         <v>323</v>
       </c>
       <c r="FA56" s="33" t="s">
-        <v>688</v>
+        <v>665</v>
       </c>
       <c r="FB56" s="4" t="s">
         <v>323</v>
@@ -25974,7 +25983,7 @@
         <v>323</v>
       </c>
       <c r="FG56" s="33" t="s">
-        <v>689</v>
+        <v>666</v>
       </c>
       <c r="FH56" s="4" t="s">
         <v>323</v>
@@ -25992,7 +26001,7 @@
         <v>323</v>
       </c>
       <c r="FM56" s="33" t="s">
-        <v>690</v>
+        <v>667</v>
       </c>
       <c r="FN56" s="4" t="s">
         <v>323</v>
@@ -26028,7 +26037,7 @@
         <v>333</v>
       </c>
       <c r="FY56" s="22" t="s">
-        <v>691</v>
+        <v>732</v>
       </c>
       <c r="FZ56" t="s">
         <v>333</v>
@@ -26046,7 +26055,7 @@
         <v>333</v>
       </c>
       <c r="GE56" s="22" t="s">
-        <v>692</v>
+        <v>733</v>
       </c>
       <c r="GF56" t="s">
         <v>333</v>
@@ -26064,7 +26073,7 @@
         <v>333</v>
       </c>
       <c r="GK56" s="22" t="s">
-        <v>693</v>
+        <v>737</v>
       </c>
       <c r="GL56" t="s">
         <v>333</v>
@@ -26100,7 +26109,7 @@
         <v>344</v>
       </c>
       <c r="GW56" s="41" t="s">
-        <v>694</v>
+        <v>668</v>
       </c>
       <c r="GX56" s="22" t="s">
         <v>344</v>
@@ -26118,7 +26127,7 @@
         <v>344</v>
       </c>
       <c r="HC56" s="41" t="s">
-        <v>695</v>
+        <v>669</v>
       </c>
       <c r="HD56" s="22" t="s">
         <v>344</v>
@@ -26136,7 +26145,7 @@
         <v>344</v>
       </c>
       <c r="HI56" s="41" t="s">
-        <v>696</v>
+        <v>670</v>
       </c>
       <c r="HJ56" s="22" t="s">
         <v>344</v>
@@ -26570,7 +26579,7 @@
         <v>314</v>
       </c>
       <c r="EE57" s="22" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
       <c r="EF57" s="30" t="s">
         <v>314</v>
@@ -26588,7 +26597,7 @@
         <v>314</v>
       </c>
       <c r="EK57" s="22" t="s">
-        <v>698</v>
+        <v>712</v>
       </c>
       <c r="EL57" s="30" t="s">
         <v>314</v>
@@ -26606,7 +26615,7 @@
         <v>314</v>
       </c>
       <c r="EQ57" s="22" t="s">
-        <v>699</v>
+        <v>714</v>
       </c>
       <c r="ER57" s="30" t="s">
         <v>314</v>
@@ -26642,7 +26651,7 @@
         <v>124</v>
       </c>
       <c r="FC57" s="33" t="s">
-        <v>700</v>
+        <v>671</v>
       </c>
       <c r="FD57" s="4" t="s">
         <v>124</v>
@@ -26660,7 +26669,7 @@
         <v>124</v>
       </c>
       <c r="FI57" s="33" t="s">
-        <v>701</v>
+        <v>672</v>
       </c>
       <c r="FJ57" s="4" t="s">
         <v>124</v>
@@ -26678,7 +26687,7 @@
         <v>124</v>
       </c>
       <c r="FO57" s="33" t="s">
-        <v>702</v>
+        <v>673</v>
       </c>
       <c r="FP57" s="4" t="s">
         <v>124</v>
@@ -26713,8 +26722,8 @@
       <c r="FZ57" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="GA57" s="34" t="s">
-        <v>703</v>
+      <c r="GA57" s="44" t="s">
+        <v>736</v>
       </c>
       <c r="GB57" s="15" t="s">
         <v>334</v>
@@ -26732,7 +26741,7 @@
         <v>334</v>
       </c>
       <c r="GG57" s="34" t="s">
-        <v>704</v>
+        <v>730</v>
       </c>
       <c r="GH57" s="15" t="s">
         <v>334</v>
@@ -26750,7 +26759,7 @@
         <v>334</v>
       </c>
       <c r="GM57" s="34" t="s">
-        <v>705</v>
+        <v>738</v>
       </c>
       <c r="GN57" s="15" t="s">
         <v>334</v>
@@ -26786,7 +26795,7 @@
         <v>345</v>
       </c>
       <c r="GY57" s="41" t="s">
-        <v>706</v>
+        <v>674</v>
       </c>
       <c r="GZ57" s="22" t="s">
         <v>345</v>
@@ -26804,7 +26813,7 @@
         <v>345</v>
       </c>
       <c r="HE57" s="41" t="s">
-        <v>707</v>
+        <v>675</v>
       </c>
       <c r="HF57" s="22" t="s">
         <v>345</v>
@@ -26822,7 +26831,7 @@
         <v>345</v>
       </c>
       <c r="HK57" s="41" t="s">
-        <v>708</v>
+        <v>676</v>
       </c>
       <c r="HL57" s="22" t="s">
         <v>345</v>
@@ -27259,7 +27268,7 @@
         <v>310</v>
       </c>
       <c r="EH58" s="22" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="EI58" s="30" t="s">
         <v>310</v>
@@ -27277,7 +27286,7 @@
         <v>310</v>
       </c>
       <c r="EN58" s="22" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="EO58" s="30" t="s">
         <v>310</v>
@@ -27313,7 +27322,7 @@
         <v>322</v>
       </c>
       <c r="EZ58" s="33" t="s">
-        <v>712</v>
+        <v>677</v>
       </c>
       <c r="FA58" s="4" t="s">
         <v>322</v>
@@ -27331,7 +27340,7 @@
         <v>322</v>
       </c>
       <c r="FF58" s="33" t="s">
-        <v>713</v>
+        <v>678</v>
       </c>
       <c r="FG58" s="4" t="s">
         <v>322</v>
@@ -27349,7 +27358,7 @@
         <v>322</v>
       </c>
       <c r="FL58" s="33" t="s">
-        <v>714</v>
+        <v>679</v>
       </c>
       <c r="FM58" s="4" t="s">
         <v>322</v>
@@ -27385,7 +27394,7 @@
         <v>332</v>
       </c>
       <c r="FX58" s="22" t="s">
-        <v>715</v>
+        <v>680</v>
       </c>
       <c r="FY58" t="s">
         <v>332</v>
@@ -27403,7 +27412,7 @@
         <v>332</v>
       </c>
       <c r="GD58" s="22" t="s">
-        <v>716</v>
+        <v>681</v>
       </c>
       <c r="GE58" t="s">
         <v>332</v>
@@ -27421,7 +27430,7 @@
         <v>332</v>
       </c>
       <c r="GJ58" s="22" t="s">
-        <v>717</v>
+        <v>682</v>
       </c>
       <c r="GK58" t="s">
         <v>332</v>
@@ -27457,7 +27466,7 @@
         <v>343</v>
       </c>
       <c r="GV58" s="41" t="s">
-        <v>718</v>
+        <v>683</v>
       </c>
       <c r="GW58" s="22" t="s">
         <v>343</v>
@@ -27475,7 +27484,7 @@
         <v>343</v>
       </c>
       <c r="HB58" s="41" t="s">
-        <v>719</v>
+        <v>684</v>
       </c>
       <c r="HC58" s="22" t="s">
         <v>343</v>
@@ -27493,7 +27502,7 @@
         <v>343</v>
       </c>
       <c r="HH58" s="41" t="s">
-        <v>720</v>
+        <v>685</v>
       </c>
       <c r="HI58" s="22" t="s">
         <v>343</v>
@@ -27927,7 +27936,7 @@
         <v>317</v>
       </c>
       <c r="ED59" s="22" t="s">
-        <v>721</v>
+        <v>686</v>
       </c>
       <c r="EE59" s="30" t="s">
         <v>317</v>
@@ -27945,7 +27954,7 @@
         <v>317</v>
       </c>
       <c r="EJ59" s="22" t="s">
-        <v>722</v>
+        <v>687</v>
       </c>
       <c r="EK59" s="30" t="s">
         <v>317</v>
@@ -27963,7 +27972,7 @@
         <v>317</v>
       </c>
       <c r="EP59" s="22" t="s">
-        <v>723</v>
+        <v>688</v>
       </c>
       <c r="EQ59" s="30" t="s">
         <v>317</v>
@@ -27999,7 +28008,7 @@
         <v>324</v>
       </c>
       <c r="FB59" s="33" t="s">
-        <v>724</v>
+        <v>689</v>
       </c>
       <c r="FC59" s="4" t="s">
         <v>324</v>
@@ -28017,7 +28026,7 @@
         <v>324</v>
       </c>
       <c r="FH59" s="33" t="s">
-        <v>725</v>
+        <v>690</v>
       </c>
       <c r="FI59" s="4" t="s">
         <v>324</v>
@@ -28035,7 +28044,7 @@
         <v>324</v>
       </c>
       <c r="FN59" s="33" t="s">
-        <v>726</v>
+        <v>691</v>
       </c>
       <c r="FO59" s="4" t="s">
         <v>324</v>
@@ -28070,8 +28079,8 @@
       <c r="FY59" t="s">
         <v>335</v>
       </c>
-      <c r="FZ59" s="22" t="s">
-        <v>727</v>
+      <c r="FZ59" s="43" t="s">
+        <v>734</v>
       </c>
       <c r="GA59" t="s">
         <v>335</v>
@@ -28089,7 +28098,7 @@
         <v>335</v>
       </c>
       <c r="GF59" s="22" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="GG59" t="s">
         <v>335</v>
@@ -28143,7 +28152,7 @@
         <v>346</v>
       </c>
       <c r="GX59" s="41" t="s">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="GY59" s="22" t="s">
         <v>346</v>
@@ -28161,7 +28170,7 @@
         <v>346</v>
       </c>
       <c r="HD59" s="41" t="s">
-        <v>731</v>
+        <v>693</v>
       </c>
       <c r="HE59" s="22" t="s">
         <v>346</v>
@@ -28179,7 +28188,7 @@
         <v>346</v>
       </c>
       <c r="HJ59" s="41" t="s">
-        <v>732</v>
+        <v>694</v>
       </c>
       <c r="HK59" s="22" t="s">
         <v>346</v>
@@ -28613,7 +28622,7 @@
         <v>319</v>
       </c>
       <c r="EF60" s="22" t="s">
-        <v>733</v>
+        <v>695</v>
       </c>
       <c r="EG60" s="30" t="s">
         <v>319</v>
@@ -28631,7 +28640,7 @@
         <v>319</v>
       </c>
       <c r="EL60" s="22" t="s">
-        <v>734</v>
+        <v>696</v>
       </c>
       <c r="EM60" s="30" t="s">
         <v>319</v>
@@ -28649,7 +28658,7 @@
         <v>319</v>
       </c>
       <c r="ER60" s="22" t="s">
-        <v>735</v>
+        <v>697</v>
       </c>
       <c r="ES60" s="30" t="s">
         <v>319</v>
@@ -28685,7 +28694,7 @@
         <v>325</v>
       </c>
       <c r="FD60" s="33" t="s">
-        <v>736</v>
+        <v>698</v>
       </c>
       <c r="FE60" s="4" t="s">
         <v>325</v>
@@ -28703,7 +28712,7 @@
         <v>325</v>
       </c>
       <c r="FJ60" s="33" t="s">
-        <v>737</v>
+        <v>699</v>
       </c>
       <c r="FK60" s="4" t="s">
         <v>325</v>
@@ -28721,7 +28730,7 @@
         <v>325</v>
       </c>
       <c r="FP60" s="33" t="s">
-        <v>738</v>
+        <v>700</v>
       </c>
       <c r="FQ60" s="4" t="s">
         <v>325</v>
@@ -28756,8 +28765,8 @@
       <c r="GA60" t="s">
         <v>336</v>
       </c>
-      <c r="GB60" s="22" t="s">
-        <v>739</v>
+      <c r="GB60" s="45" t="s">
+        <v>701</v>
       </c>
       <c r="GC60" t="s">
         <v>336</v>
@@ -28775,7 +28784,7 @@
         <v>336</v>
       </c>
       <c r="GH60" s="22" t="s">
-        <v>740</v>
+        <v>702</v>
       </c>
       <c r="GI60" t="s">
         <v>336</v>
@@ -28793,7 +28802,7 @@
         <v>336</v>
       </c>
       <c r="GN60" s="22" t="s">
-        <v>741</v>
+        <v>703</v>
       </c>
       <c r="GO60" t="s">
         <v>336</v>
@@ -28829,7 +28838,7 @@
         <v>347</v>
       </c>
       <c r="GZ60" s="41" t="s">
-        <v>742</v>
+        <v>704</v>
       </c>
       <c r="HA60" s="22" t="s">
         <v>347</v>
@@ -28847,7 +28856,7 @@
         <v>347</v>
       </c>
       <c r="HF60" s="41" t="s">
-        <v>743</v>
+        <v>705</v>
       </c>
       <c r="HG60" s="22" t="s">
         <v>347</v>
@@ -28865,7 +28874,7 @@
         <v>347</v>
       </c>
       <c r="HL60" s="41" t="s">
-        <v>744</v>
+        <v>706</v>
       </c>
       <c r="HM60" s="22" t="s">
         <v>347</v>

</xml_diff>

<commit_message>
changes to cattle code and scenario file
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8AE0B4-426D-0D49-872D-93CD08E0D8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763FBADE-CE58-9E42-8A0D-222C9C72A79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="26820" windowHeight="16300" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="26820" windowHeight="16100" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2970,8 +2970,8 @@
   <dimension ref="A1:IH121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EF1" sqref="EF1:IE1048576"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG1" sqref="AG1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>